<commit_message>
Fix duplicate id in anomaly example of employees
</commit_message>
<xml_diff>
--- a/assets/C02/Anomalies.xlsx
+++ b/assets/C02/Anomalies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -407,6 +407,9 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -423,9 +426,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -676,52 +676,52 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B3:E9" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B3:E9" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="B3:E9"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="course" dataDxfId="23"/>
-    <tableColumn id="2" name="semesterID" dataDxfId="22"/>
-    <tableColumn id="3" name="places" dataDxfId="21"/>
-    <tableColumn id="4" name="courseName" dataDxfId="20"/>
+    <tableColumn id="1" name="course" dataDxfId="21"/>
+    <tableColumn id="2" name="semesterID" dataDxfId="20"/>
+    <tableColumn id="3" name="places" dataDxfId="19"/>
+    <tableColumn id="4" name="courseName" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="G3:J8" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="G3:J8" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="G3:J8"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="courseID [PK]" dataDxfId="10"/>
-    <tableColumn id="2" name="semesterID [PK]" dataDxfId="9"/>
-    <tableColumn id="3" name="places" dataDxfId="8"/>
-    <tableColumn id="4" name="courseName" dataDxfId="7"/>
+    <tableColumn id="1" name="courseID [PK]" dataDxfId="15"/>
+    <tableColumn id="2" name="semesterID [PK]" dataDxfId="14"/>
+    <tableColumn id="3" name="places" dataDxfId="13"/>
+    <tableColumn id="4" name="courseName" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="M3:Q8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="M3:Q8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="M3:Q8"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="courseID [PK]" dataDxfId="17"/>
-    <tableColumn id="2" name="semesterID [PK]" dataDxfId="16"/>
-    <tableColumn id="3" name="places" dataDxfId="15"/>
-    <tableColumn id="4" name="TeacherID" dataDxfId="14"/>
-    <tableColumn id="5" name="TeacherName" dataDxfId="13"/>
+    <tableColumn id="1" name="courseID [PK]" dataDxfId="9"/>
+    <tableColumn id="2" name="semesterID [PK]" dataDxfId="8"/>
+    <tableColumn id="3" name="places" dataDxfId="7"/>
+    <tableColumn id="4" name="TeacherID" dataDxfId="6"/>
+    <tableColumn id="5" name="TeacherName" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="S3:U10" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="S3:U10" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="S3:U10"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="studentID" dataDxfId="4"/>
-    <tableColumn id="2" name="SSN" dataDxfId="3"/>
-    <tableColumn id="3" name="courseID" dataDxfId="2"/>
+    <tableColumn id="1" name="studentID" dataDxfId="2"/>
+    <tableColumn id="2" name="SSN" dataDxfId="1"/>
+    <tableColumn id="3" name="courseID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:E44"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,20 +1036,20 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="H4" s="10" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="H4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1117,7 +1117,7 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -1273,20 +1273,20 @@
     </row>
     <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
-      <c r="H19" s="10" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="H19" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="13"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
@@ -1354,7 +1354,7 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>5</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>7</v>
@@ -1547,8 +1547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,31 +1951,31 @@
     </row>
     <row r="25" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M25" s="1"/>
-      <c r="N25" s="13"/>
+      <c r="N25" s="7"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
     <row r="26" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M26" s="1"/>
-      <c r="N26" s="13"/>
+      <c r="N26" s="7"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
     <row r="27" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M27" s="1"/>
-      <c r="N27" s="13"/>
+      <c r="N27" s="7"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
     <row r="28" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M28" s="1"/>
-      <c r="N28" s="13"/>
+      <c r="N28" s="7"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
     <row r="29" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M29" s="1"/>
-      <c r="N29" s="13"/>
+      <c r="N29" s="7"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>

</xml_diff>